<commit_message>
20231213 Commit after Excel Download included
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevWork\EEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D80CC3C-15C8-44AD-8C46-7533A1E1EFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B655D1-975F-4846-B85B-BB20C083BC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="210">
   <si>
     <t>Capital Cost Baseline</t>
   </si>
@@ -762,9 +762,6 @@
   </si>
   <si>
     <t>CO2 Emissions for Diesel</t>
-  </si>
-  <si>
-    <t>from PCL 1.15</t>
   </si>
   <si>
     <t>Rs/MWh</t>
@@ -9610,7 +9607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1DE934-23F3-4414-B95B-145CF3421268}">
   <dimension ref="A3:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -11096,8 +11093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D27CD2-E810-4FE6-87F8-09242D0DB167}">
   <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11105,9 +11102,10 @@
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>58</v>
       </c>
@@ -11118,7 +11116,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>73</v>
       </c>
@@ -11132,7 +11130,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>74</v>
       </c>
@@ -11144,19 +11142,23 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>75</v>
       </c>
       <c r="B5" s="92">
-        <f>8000</f>
-        <v>8000</v>
+        <f>29.9*1000</f>
+        <v>29900</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>B5/B3</f>
+        <v>24.916666666666668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>76</v>
       </c>
@@ -11165,7 +11167,7 @@
       </c>
       <c r="C6" s="19"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>203</v>
       </c>
@@ -11176,12 +11178,13 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="72">
-        <v>3900</v>
+        <f>15.61*284</f>
+        <v>4433.24</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>43</v>
@@ -11190,7 +11193,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>67</v>
       </c>
@@ -11202,21 +11205,21 @@
       </c>
       <c r="D9" s="90"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="91">
-        <v>14657</v>
+        <f>B8*D5</f>
+        <v>110461.56333333334</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="83" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="83"/>
+      <c r="F10" s="90"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>49</v>
       </c>
@@ -11225,7 +11228,7 @@
       </c>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>204</v>
       </c>
@@ -11236,12 +11239,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>77</v>
       </c>
       <c r="B13" s="72">
-        <v>198826.33</v>
+        <v>240000</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>162</v>
@@ -11250,7 +11253,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>78</v>
       </c>
@@ -11261,18 +11264,18 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>79</v>
       </c>
       <c r="B15" s="91">
-        <v>26923</v>
+        <v>29900</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>80</v>
       </c>
@@ -11325,7 +11328,7 @@
       </c>
       <c r="B20" s="54">
         <f>B15</f>
-        <v>26923</v>
+        <v>29900</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>39</v>
@@ -11382,7 +11385,7 @@
         <v>47</v>
       </c>
       <c r="B25" s="52">
-        <v>39000</v>
+        <v>40000</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>39</v>
@@ -11437,10 +11440,10 @@
         <v>71</v>
       </c>
       <c r="B30" s="52">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -11760,15 +11763,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ad74739f-b6c5-48e8-a4a2-e396fec78e6b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="78d2dcdf-d17c-4586-ad68-d792bc06c6b5" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="ad74739f-b6c5-48e8-a4a2-e396fec78e6b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12027,27 +12027,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ad74739f-b6c5-48e8-a4a2-e396fec78e6b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="78d2dcdf-d17c-4586-ad68-d792bc06c6b5" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="ad74739f-b6c5-48e8-a4a2-e396fec78e6b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CC7F60-97FA-47D2-813C-DE1DF9F0EBEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A7ADAC-11AC-4699-B4EA-2CE8EDD8A75B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="78d2dcdf-d17c-4586-ad68-d792bc06c6b5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ad74739f-b6c5-48e8-a4a2-e396fec78e6b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12072,9 +12066,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A7ADAC-11AC-4699-B4EA-2CE8EDD8A75B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CC7F60-97FA-47D2-813C-DE1DF9F0EBEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="78d2dcdf-d17c-4586-ad68-d792bc06c6b5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ad74739f-b6c5-48e8-a4a2-e396fec78e6b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
20231213 optimized for download.
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevWork\EEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B655D1-975F-4846-B85B-BB20C083BC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A39960-BB98-4839-8298-ED191B38A3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19725" windowHeight="11760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind" sheetId="2" r:id="rId1"/>
@@ -11093,8 +11093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D27CD2-E810-4FE6-87F8-09242D0DB167}">
   <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11269,7 +11269,7 @@
         <v>79</v>
       </c>
       <c r="B15" s="91">
-        <v>29900</v>
+        <v>61479</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>39</v>
@@ -11328,7 +11328,7 @@
       </c>
       <c r="B20" s="54">
         <f>B15</f>
-        <v>29900</v>
+        <v>61479</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>39</v>
@@ -11763,12 +11763,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ad74739f-b6c5-48e8-a4a2-e396fec78e6b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="78d2dcdf-d17c-4586-ad68-d792bc06c6b5" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="ad74739f-b6c5-48e8-a4a2-e396fec78e6b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12027,21 +12030,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ad74739f-b6c5-48e8-a4a2-e396fec78e6b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="78d2dcdf-d17c-4586-ad68-d792bc06c6b5" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="ad74739f-b6c5-48e8-a4a2-e396fec78e6b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A7ADAC-11AC-4699-B4EA-2CE8EDD8A75B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CC7F60-97FA-47D2-813C-DE1DF9F0EBEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="78d2dcdf-d17c-4586-ad68-d792bc06c6b5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ad74739f-b6c5-48e8-a4a2-e396fec78e6b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12066,18 +12075,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CC7F60-97FA-47D2-813C-DE1DF9F0EBEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70A7ADAC-11AC-4699-B4EA-2CE8EDD8A75B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="78d2dcdf-d17c-4586-ad68-d792bc06c6b5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ad74739f-b6c5-48e8-a4a2-e396fec78e6b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>